<commit_message>
Removed required 'min' & 'sec' event log attributes
</commit_message>
<xml_diff>
--- a/test/resources/AutoCalc_Soccer_EventLog.invalid.xlsx
+++ b/test/resources/AutoCalc_Soccer_EventLog.invalid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EventType" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="240">
   <si>
     <t>Half 1</t>
   </si>
@@ -603,12 +603,6 @@
     <t>Head</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>sec</t>
-  </si>
-  <si>
     <t>Standart</t>
   </si>
   <si>
@@ -1136,6 +1130,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1157,12 +1157,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7805,7 +7799,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -8138,7 +8132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8148,7 +8142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40:D55"/>
     </sheetView>
   </sheetViews>
@@ -8163,16 +8157,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8183,7 +8177,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>20</v>
@@ -8197,7 +8191,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
@@ -8211,7 +8205,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>186</v>
@@ -8225,7 +8219,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>187</v>
@@ -8239,7 +8233,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>188</v>
@@ -8253,7 +8247,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>189</v>
@@ -8267,10 +8261,10 @@
         <v>43</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8281,7 +8275,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>53</v>
@@ -8295,7 +8289,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>17</v>
@@ -8309,10 +8303,10 @@
         <v>43</v>
       </c>
       <c r="C11" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -8323,7 +8317,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>190</v>
@@ -8337,10 +8331,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1">
@@ -8351,18 +8345,18 @@
         <v>43</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" thickTop="1">
       <c r="B15" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>20</v>
@@ -8370,10 +8364,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>21</v>
@@ -8381,10 +8375,10 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>186</v>
@@ -8392,10 +8386,10 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>187</v>
@@ -8403,10 +8397,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>188</v>
@@ -8414,10 +8408,10 @@
     </row>
     <row r="20" spans="2:4" ht="15" thickBot="1">
       <c r="B20" s="44" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>189</v>
@@ -8428,7 +8422,7 @@
         <v>185</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D21" s="43" t="s">
         <v>20</v>
@@ -8439,7 +8433,7 @@
         <v>185</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>21</v>
@@ -8450,7 +8444,7 @@
         <v>185</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>186</v>
@@ -8461,7 +8455,7 @@
         <v>185</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>187</v>
@@ -8472,7 +8466,7 @@
         <v>185</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>188</v>
@@ -8483,7 +8477,7 @@
         <v>185</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D26" s="44" t="s">
         <v>189</v>
@@ -8494,7 +8488,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D27" s="43" t="s">
         <v>20</v>
@@ -8505,7 +8499,7 @@
         <v>53</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -8516,7 +8510,7 @@
         <v>53</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>186</v>
@@ -8527,7 +8521,7 @@
         <v>53</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>187</v>
@@ -8538,7 +8532,7 @@
         <v>53</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>188</v>
@@ -8549,7 +8543,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D32" s="44" t="s">
         <v>189</v>
@@ -8560,7 +8554,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>20</v>
@@ -8571,7 +8565,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>21</v>
@@ -8582,7 +8576,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>186</v>
@@ -8593,7 +8587,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>187</v>
@@ -8604,7 +8598,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>188</v>
@@ -8615,7 +8609,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>189</v>
@@ -8626,186 +8620,186 @@
         <v>17</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D39" s="44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15" thickTop="1">
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="54" t="s">
         <v>186</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="54" t="s">
         <v>186</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="54" t="s">
         <v>187</v>
       </c>
       <c r="C42" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="54" t="s">
         <v>187</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="54" t="s">
         <v>188</v>
       </c>
       <c r="C44" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="54" t="s">
         <v>188</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="2:4">
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="54" t="s">
         <v>189</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="54" t="s">
         <v>189</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="61" t="s">
-        <v>240</v>
+      <c r="B48" s="54" t="s">
+        <v>238</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="61" t="s">
-        <v>240</v>
+      <c r="B49" s="54" t="s">
+        <v>238</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="61" t="s">
-        <v>241</v>
+      <c r="B50" s="54" t="s">
+        <v>239</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="61" t="s">
-        <v>241</v>
+      <c r="B51" s="54" t="s">
+        <v>239</v>
       </c>
       <c r="C51" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="61" t="s">
-        <v>221</v>
+      <c r="B52" s="54" t="s">
+        <v>219</v>
       </c>
       <c r="C52" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" s="61" t="s">
-        <v>221</v>
+      <c r="B53" s="54" t="s">
+        <v>219</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="61" t="s">
-        <v>225</v>
+      <c r="B54" s="54" t="s">
+        <v>223</v>
       </c>
       <c r="C54" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" s="61" t="s">
-        <v>225</v>
+      <c r="B55" s="54" t="s">
+        <v>223</v>
       </c>
       <c r="C55" s="47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -8839,66 +8833,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="1" customWidth="1"/>
-    <col min="3" max="14" width="16.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12" style="1" customWidth="1"/>
-    <col min="20" max="20" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="12" width="16.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>197</v>
-      </c>
       <c r="E1" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="47" t="s">
-        <v>228</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="J1" s="42"/>
+        <v>237</v>
+      </c>
+      <c r="H1" s="42"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
       <c r="P1" s="33"/>
       <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -8906,585 +8892,483 @@
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="33"/>
       <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="33">
-        <v>0</v>
-      </c>
-      <c r="B3" s="32">
-        <v>0</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>225</v>
-      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="J3" s="42"/>
+      <c r="G3" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H3" s="42"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="32">
-        <v>0</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>205</v>
-      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="32">
-        <v>0</v>
-      </c>
-      <c r="C5" s="33" t="s">
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="I5" s="32" t="s">
-        <v>205</v>
-      </c>
+      <c r="G5" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="1">
-        <v>12</v>
-      </c>
-      <c r="B6" s="32">
-        <v>32</v>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="1">
-        <v>26</v>
-      </c>
-      <c r="B7" s="32">
-        <v>55</v>
-      </c>
-      <c r="C7" s="32" t="s">
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="1">
-        <v>27</v>
-      </c>
-      <c r="B8" s="32">
-        <v>23</v>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="1">
-        <v>30</v>
-      </c>
-      <c r="B9" s="32">
-        <v>44</v>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="1">
-        <v>33</v>
-      </c>
-      <c r="B10" s="32">
-        <v>23</v>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="1">
-        <v>45</v>
-      </c>
-      <c r="B11" s="32">
-        <v>0</v>
-      </c>
-      <c r="C11" s="33" t="s">
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="I11" s="32" t="s">
-        <v>206</v>
-      </c>
+      <c r="G11" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="1">
-        <v>46</v>
-      </c>
-      <c r="B12" s="32">
-        <v>77</v>
-      </c>
-      <c r="C12" s="33" t="s">
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="I12" s="32" t="s">
-        <v>205</v>
-      </c>
+      <c r="G12" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="1">
-        <v>51</v>
-      </c>
-      <c r="B13" s="32">
-        <v>11</v>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="1">
-        <v>52</v>
-      </c>
-      <c r="B14" s="32">
-        <v>1</v>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="1">
-        <v>62</v>
-      </c>
-      <c r="B15" s="32">
-        <v>2</v>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="1">
-        <v>62</v>
-      </c>
-      <c r="B16" s="32">
-        <v>11</v>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I16" s="32"/>
+        <v>192</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="1">
-        <v>91</v>
-      </c>
-      <c r="B17" s="32">
-        <v>32</v>
-      </c>
-      <c r="C17" s="33" t="s">
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="I17" s="32" t="s">
-        <v>206</v>
-      </c>
+      <c r="G17" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="1">
-        <v>92</v>
-      </c>
-      <c r="B18" s="32">
-        <v>0</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="J18" s="42"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="42"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="1">
-        <v>92</v>
-      </c>
-      <c r="B19" s="32">
-        <v>0</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>225</v>
-      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="32" t="s">
-        <v>206</v>
-      </c>
+      <c r="G19" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="42"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15">
+    </row>
+    <row r="21" spans="1:13">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15">
+    </row>
+    <row r="22" spans="1:13">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15">
+    </row>
+    <row r="23" spans="1:13">
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15">
+    </row>
+    <row r="24" spans="1:13">
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15">
+    </row>
+    <row r="25" spans="1:13">
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15">
+    </row>
+    <row r="26" spans="1:13">
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15">
+    </row>
+    <row r="27" spans="1:13">
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15">
+    </row>
+    <row r="28" spans="1:13">
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:15">
+    </row>
+    <row r="29" spans="1:13">
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15">
+    </row>
+    <row r="30" spans="1:13">
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15">
+    </row>
+    <row r="31" spans="1:13">
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="1:15">
+    </row>
+    <row r="32" spans="1:13">
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
       <c r="J32" s="42"/>
       <c r="K32" s="42"/>
       <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="5:14">
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="3:12">
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
@@ -9493,10 +9377,10 @@
       <c r="J33" s="33"/>
       <c r="K33" s="33"/>
       <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-    </row>
-    <row r="34" spans="5:14">
+    </row>
+    <row r="34" spans="3:12">
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
@@ -9505,10 +9389,10 @@
       <c r="J34" s="33"/>
       <c r="K34" s="33"/>
       <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-    </row>
-    <row r="35" spans="5:14">
+    </row>
+    <row r="35" spans="3:12">
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
@@ -9517,10 +9401,10 @@
       <c r="J35" s="33"/>
       <c r="K35" s="33"/>
       <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-    </row>
-    <row r="36" spans="5:14">
+    </row>
+    <row r="36" spans="3:12">
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="33"/>
       <c r="G36" s="33"/>
@@ -9529,10 +9413,10 @@
       <c r="J36" s="33"/>
       <c r="K36" s="33"/>
       <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-    </row>
-    <row r="37" spans="5:14">
+    </row>
+    <row r="37" spans="3:12">
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="33"/>
       <c r="G37" s="33"/>
@@ -9541,10 +9425,10 @@
       <c r="J37" s="33"/>
       <c r="K37" s="33"/>
       <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-    </row>
-    <row r="38" spans="5:14">
+    </row>
+    <row r="38" spans="3:12">
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="33"/>
       <c r="G38" s="33"/>
@@ -9553,10 +9437,10 @@
       <c r="J38" s="33"/>
       <c r="K38" s="33"/>
       <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-    </row>
-    <row r="39" spans="5:14">
+    </row>
+    <row r="39" spans="3:12">
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
       <c r="G39" s="33"/>
@@ -9565,10 +9449,10 @@
       <c r="J39" s="33"/>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-    </row>
-    <row r="40" spans="5:14">
+    </row>
+    <row r="40" spans="3:12">
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
@@ -9577,10 +9461,10 @@
       <c r="J40" s="33"/>
       <c r="K40" s="33"/>
       <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-    </row>
-    <row r="41" spans="5:14">
+    </row>
+    <row r="41" spans="3:12">
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
@@ -9589,10 +9473,10 @@
       <c r="J41" s="33"/>
       <c r="K41" s="33"/>
       <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-    </row>
-    <row r="42" spans="5:14">
+    </row>
+    <row r="42" spans="3:12">
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -9601,10 +9485,10 @@
       <c r="J42" s="33"/>
       <c r="K42" s="33"/>
       <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-    </row>
-    <row r="43" spans="5:14">
+    </row>
+    <row r="43" spans="3:12">
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
@@ -9613,10 +9497,10 @@
       <c r="J43" s="33"/>
       <c r="K43" s="33"/>
       <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="33"/>
-    </row>
-    <row r="44" spans="5:14">
+    </row>
+    <row r="44" spans="3:12">
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
@@ -9625,10 +9509,10 @@
       <c r="J44" s="33"/>
       <c r="K44" s="33"/>
       <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-    </row>
-    <row r="45" spans="5:14">
+    </row>
+    <row r="45" spans="3:12">
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
@@ -9637,10 +9521,10 @@
       <c r="J45" s="33"/>
       <c r="K45" s="33"/>
       <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-    </row>
-    <row r="46" spans="5:14">
+    </row>
+    <row r="46" spans="3:12">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="33"/>
       <c r="G46" s="33"/>
@@ -9649,10 +9533,10 @@
       <c r="J46" s="33"/>
       <c r="K46" s="33"/>
       <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="33"/>
-    </row>
-    <row r="47" spans="5:14">
+    </row>
+    <row r="47" spans="3:12">
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="33"/>
       <c r="G47" s="33"/>
@@ -9661,10 +9545,10 @@
       <c r="J47" s="33"/>
       <c r="K47" s="33"/>
       <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-    </row>
-    <row r="48" spans="5:14">
+    </row>
+    <row r="48" spans="3:12">
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
@@ -9673,10 +9557,10 @@
       <c r="J48" s="33"/>
       <c r="K48" s="33"/>
       <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
-      <c r="N48" s="33"/>
-    </row>
-    <row r="49" spans="5:14">
+    </row>
+    <row r="49" spans="3:12">
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="33"/>
       <c r="G49" s="33"/>
@@ -9685,10 +9569,10 @@
       <c r="J49" s="33"/>
       <c r="K49" s="33"/>
       <c r="L49" s="33"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="33"/>
-    </row>
-    <row r="50" spans="5:14">
+    </row>
+    <row r="50" spans="3:12">
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
@@ -9697,10 +9581,10 @@
       <c r="J50" s="33"/>
       <c r="K50" s="33"/>
       <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-    </row>
-    <row r="51" spans="5:14">
+    </row>
+    <row r="51" spans="3:12">
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="33"/>
       <c r="G51" s="33"/>
@@ -9709,10 +9593,10 @@
       <c r="J51" s="33"/>
       <c r="K51" s="33"/>
       <c r="L51" s="33"/>
-      <c r="M51" s="33"/>
-      <c r="N51" s="33"/>
-    </row>
-    <row r="52" spans="5:14">
+    </row>
+    <row r="52" spans="3:12">
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
@@ -9721,10 +9605,10 @@
       <c r="J52" s="33"/>
       <c r="K52" s="33"/>
       <c r="L52" s="33"/>
-      <c r="M52" s="33"/>
-      <c r="N52" s="33"/>
-    </row>
-    <row r="53" spans="5:14">
+    </row>
+    <row r="53" spans="3:12">
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="33"/>
       <c r="G53" s="33"/>
@@ -9733,10 +9617,10 @@
       <c r="J53" s="33"/>
       <c r="K53" s="33"/>
       <c r="L53" s="33"/>
-      <c r="M53" s="33"/>
-      <c r="N53" s="33"/>
-    </row>
-    <row r="54" spans="5:14">
+    </row>
+    <row r="54" spans="3:12">
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="33"/>
       <c r="G54" s="33"/>
@@ -9745,10 +9629,10 @@
       <c r="J54" s="33"/>
       <c r="K54" s="33"/>
       <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-    </row>
-    <row r="55" spans="5:14">
+    </row>
+    <row r="55" spans="3:12">
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="33"/>
       <c r="G55" s="33"/>
@@ -9757,10 +9641,10 @@
       <c r="J55" s="33"/>
       <c r="K55" s="33"/>
       <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
-    </row>
-    <row r="57" spans="5:14">
+    </row>
+    <row r="57" spans="3:12">
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="33"/>
       <c r="G57" s="33"/>
       <c r="H57" s="33"/>
@@ -9768,10 +9652,10 @@
       <c r="J57" s="33"/>
       <c r="K57" s="33"/>
       <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-    </row>
-    <row r="58" spans="5:14">
+    </row>
+    <row r="58" spans="3:12">
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
       <c r="E58" s="33"/>
       <c r="F58" s="33"/>
       <c r="G58" s="33"/>
@@ -9780,10 +9664,10 @@
       <c r="J58" s="33"/>
       <c r="K58" s="33"/>
       <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-    </row>
-    <row r="59" spans="5:14">
+    </row>
+    <row r="59" spans="3:12">
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
       <c r="E59" s="33"/>
       <c r="F59" s="33"/>
       <c r="G59" s="33"/>
@@ -9792,10 +9676,10 @@
       <c r="J59" s="33"/>
       <c r="K59" s="33"/>
       <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-    </row>
-    <row r="60" spans="5:14">
+    </row>
+    <row r="60" spans="3:12">
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
       <c r="F60" s="33"/>
       <c r="G60" s="33"/>
       <c r="H60" s="33"/>
@@ -9803,10 +9687,10 @@
       <c r="J60" s="33"/>
       <c r="K60" s="33"/>
       <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-    </row>
-    <row r="61" spans="5:14">
+    </row>
+    <row r="61" spans="3:12">
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
       <c r="F61" s="33"/>
       <c r="G61" s="33"/>
       <c r="H61" s="33"/>
@@ -9814,10 +9698,10 @@
       <c r="J61" s="33"/>
       <c r="K61" s="33"/>
       <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
-    </row>
-    <row r="62" spans="5:14">
+    </row>
+    <row r="62" spans="3:12">
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
       <c r="F62" s="33"/>
       <c r="G62" s="33"/>
       <c r="H62" s="33"/>
@@ -9825,10 +9709,10 @@
       <c r="J62" s="33"/>
       <c r="K62" s="33"/>
       <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-    </row>
-    <row r="63" spans="5:14">
+    </row>
+    <row r="63" spans="3:12">
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
       <c r="F63" s="33"/>
       <c r="G63" s="33"/>
       <c r="H63" s="33"/>
@@ -9836,10 +9720,10 @@
       <c r="J63" s="33"/>
       <c r="K63" s="33"/>
       <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-    </row>
-    <row r="64" spans="5:14">
+    </row>
+    <row r="64" spans="3:12">
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
       <c r="F64" s="33"/>
       <c r="G64" s="33"/>
       <c r="H64" s="33"/>
@@ -9847,10 +9731,10 @@
       <c r="J64" s="33"/>
       <c r="K64" s="33"/>
       <c r="L64" s="33"/>
-      <c r="M64" s="33"/>
-      <c r="N64" s="33"/>
-    </row>
-    <row r="65" spans="6:14">
+    </row>
+    <row r="65" spans="4:12">
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
       <c r="H65" s="33"/>
@@ -9858,10 +9742,10 @@
       <c r="J65" s="33"/>
       <c r="K65" s="33"/>
       <c r="L65" s="33"/>
-      <c r="M65" s="33"/>
-      <c r="N65" s="33"/>
-    </row>
-    <row r="66" spans="6:14">
+    </row>
+    <row r="66" spans="4:12">
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
       <c r="F66" s="33"/>
       <c r="G66" s="33"/>
       <c r="H66" s="33"/>
@@ -9869,10 +9753,10 @@
       <c r="J66" s="33"/>
       <c r="K66" s="33"/>
       <c r="L66" s="33"/>
-      <c r="M66" s="33"/>
-      <c r="N66" s="33"/>
-    </row>
-    <row r="67" spans="6:14">
+    </row>
+    <row r="67" spans="4:12">
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
       <c r="F67" s="33"/>
       <c r="G67" s="33"/>
       <c r="H67" s="33"/>
@@ -9880,10 +9764,10 @@
       <c r="J67" s="33"/>
       <c r="K67" s="33"/>
       <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-    </row>
-    <row r="68" spans="6:14">
+    </row>
+    <row r="68" spans="4:12">
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
       <c r="F68" s="33"/>
       <c r="G68" s="33"/>
       <c r="H68" s="33"/>
@@ -9891,13 +9775,8 @@
       <c r="J68" s="33"/>
       <c r="K68" s="33"/>
       <c r="L68" s="33"/>
-      <c r="M68" s="33"/>
-      <c r="N68" s="33"/>
     </row>
   </sheetData>
-  <sortState ref="A2:P64">
-    <sortCondition ref="A1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -9942,10 +9821,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="37" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B4" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal")</f>
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
@@ -9956,7 +9835,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team2")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team2")</f>
         <v>2</v>
       </c>
       <c r="C5" s="2"/>
@@ -9967,7 +9846,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team1")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team1")</f>
         <v>2</v>
       </c>
       <c r="C6" s="2"/>
@@ -9981,10 +9860,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B8" s="2">
-        <f>COUNTIFS(EventLog!C:C,"YellowCard")</f>
+        <f>COUNTIFS(EventLog!A:A,"YellowCard")</f>
         <v>1</v>
       </c>
       <c r="C8" s="2"/>
@@ -9992,10 +9871,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B9" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Corner")</f>
+        <f>COUNTIFS(EventLog!A:A,"Corner")</f>
         <v>2</v>
       </c>
       <c r="C9" s="2"/>
@@ -10009,10 +9888,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B11" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team1", EventLog!E:E,"Half1")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team1", EventLog!C:C,"Half1")</f>
         <v>1</v>
       </c>
       <c r="C11" s="2"/>
@@ -10020,10 +9899,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B12" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team2", EventLog!E:E,"Half1")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team2", EventLog!C:C,"Half1")</f>
         <v>1</v>
       </c>
       <c r="C12" s="2"/>
@@ -10037,10 +9916,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B14" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team1", EventLog!E:E,"Half2")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team1", EventLog!C:C,"Half2")</f>
         <v>1</v>
       </c>
       <c r="C14" s="2"/>
@@ -10048,10 +9927,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",EventLog!D:D,"Team2", EventLog!E:E,"Half2")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team2", EventLog!C:C,"Half2")</f>
         <v>1</v>
       </c>
       <c r="C15" s="2"/>
@@ -10065,10 +9944,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B17" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",G:G, "&lt;&gt;")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",G:G, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="C17" s="2"/>
@@ -10082,10 +9961,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="37" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B19" s="2">
-        <f>COUNTIFS(EventLog!C:C,"Goal",H:H, "Head")</f>
+        <f>COUNTIFS(EventLog!A:A,"Goal",H:H, "Head")</f>
         <v>0</v>
       </c>
       <c r="C19" s="2"/>
@@ -10099,10 +9978,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2" t="b">
-        <f>IF(COUNTIFS(EventLog!C:C,"Goal",EventLog!E:E,"Half1",B:B,"&gt;0",B:B,"&lt;15"), TRUE,FALSE)</f>
+        <f>IF(COUNTIFS(EventLog!A:A,"Goal",EventLog!C:C,"Half1",B:B,"&gt;0",B:B,"&lt;15"), TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C21" s="2"/>
@@ -10110,10 +9989,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2" t="b">
-        <f>IF(COUNTIFS(EventLog!C:C,"Goal",EventLog!E:E,"Half1",B:B,"&gt;15",B:B,"&lt;30"), TRUE,FALSE)</f>
+        <f>IF(COUNTIFS(EventLog!A:A,"Goal",EventLog!C:C,"Half1",B:B,"&gt;15",B:B,"&lt;30"), TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C22" s="2"/>
@@ -10127,10 +10006,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B24" s="2" t="b">
-        <f>COUNTIFS(EventLog!C:C,"Match",EventLog!I:I,"stop")&gt;0</f>
+        <f>COUNTIFS(EventLog!A:A,"Match",EventLog!G:G,"stop")&gt;0</f>
         <v>1</v>
       </c>
       <c r="C24" s="2"/>
@@ -10138,10 +10017,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B25" s="2" t="b">
-        <f>COUNTIFS(EventLog!C:C,"Half1",EventLog!I:I,"stop")&gt;0</f>
+        <f>COUNTIFS(EventLog!A:A,"Half1",EventLog!G:G,"stop")&gt;0</f>
         <v>1</v>
       </c>
       <c r="C25" s="2"/>
@@ -10155,22 +10034,22 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="B27" s="2" t="b">
-        <f>0&lt;INDEX(EventLog!A:A,MATCH("Goal",EventLog!C:C,0))&lt;15</f>
-        <v>0</v>
+        <v>217</v>
+      </c>
+      <c r="B27" s="2" t="e">
+        <f>0&lt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0))&lt;15</f>
+        <v>#REF!</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="38"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="B28" s="2" t="b">
-        <f>AND(15&lt;INDEX(EventLog!A:A,MATCH("Goal",EventLog!C:C,0)),30&gt;INDEX(EventLog!A:A,MATCH("Goal",EventLog!C:C,0)))</f>
-        <v>1</v>
+        <v>218</v>
+      </c>
+      <c r="B28" s="2" t="e">
+        <f>AND(15&lt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0)),30&gt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0)))</f>
+        <v>#REF!</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="38"/>
@@ -10183,10 +10062,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f t="array" ref="B30">INDEX(EventLog!D:D,SMALL(IF(EventLog!C:C="Goal",ROW(EventLog!C:C),""),2))</f>
+        <f t="array" ref="B30">INDEX(EventLog!B:B,SMALL(IF(EventLog!A:A="Goal",ROW(EventLog!A:A),""),2))</f>
         <v>Team1</v>
       </c>
       <c r="C30" s="2"/>
@@ -10194,11 +10073,11 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="array" ref="B31">INDEX(EventLog!A:A,SMALL(IF(EventLog!C:C="Goal",ROW(EventLog!C:C),""),3))</f>
-        <v>52</v>
+        <v>225</v>
+      </c>
+      <c r="B31" s="2" t="e">
+        <f t="array" ref="B31">INDEX(EventLog!#REF!,SMALL(IF(EventLog!A:A="Goal",ROW(EventLog!A:A),""),3))</f>
+        <v>#REF!</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="38"/>
@@ -10261,32 +10140,32 @@
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="10"/>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53" t="s">
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="Z1" s="51" t="s">
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="Z1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="51"/>
+      <c r="AA1" s="55"/>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" t="s">
@@ -10343,10 +10222,10 @@
       <c r="S2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="52" t="s">
+      <c r="Z2" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="52"/>
+      <c r="AA2" s="56"/>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" t="s">
@@ -12390,109 +12269,109 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="58" t="s">
+      <c r="C4" t="s">
         <v>232</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>233</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>234</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>235</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>236</v>
       </c>
-      <c r="F4" t="s">
-        <v>237</v>
-      </c>
-      <c r="G4" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="53">
         <v>468</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="53">
         <v>10</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="53">
         <v>315</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60">
+      <c r="E5" s="53"/>
+      <c r="F5" s="53">
         <v>5</v>
       </c>
-      <c r="G5" s="60">
+      <c r="G5" s="53">
         <v>798</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53">
+        <v>1</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53">
+        <v>1</v>
+      </c>
+      <c r="F7" s="53">
+        <v>6</v>
+      </c>
+      <c r="G7" s="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60">
-        <v>1</v>
-      </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60">
-        <v>1</v>
-      </c>
-      <c r="F7" s="60">
-        <v>6</v>
-      </c>
-      <c r="G7" s="60">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="B8" s="60">
+      <c r="B8" s="53">
         <v>468</v>
       </c>
-      <c r="C8" s="60">
+      <c r="C8" s="53">
         <v>10</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="53">
         <v>315</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="53">
         <v>2</v>
       </c>
-      <c r="F8" s="60">
+      <c r="F8" s="53">
         <v>11</v>
       </c>
-      <c r="G8" s="60">
+      <c r="G8" s="53">
         <v>806</v>
       </c>
     </row>
@@ -30192,7 +30071,7 @@
       </c>
       <c r="E806" s="29"/>
       <c r="F806" t="e">
-        <f>AND(COUNTIFS(EventLog!#REF!,"Goal",EventLog!Q:Q,"&gt;61"),COUNTIFS(EventLog!#REF!,"Goal",EventLog!Q:Q,"&lt;75"))</f>
+        <f>AND(COUNTIFS(EventLog!#REF!,"Goal",EventLog!O:O,"&gt;61"),COUNTIFS(EventLog!#REF!,"Goal",EventLog!O:O,"&lt;75"))</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -30214,7 +30093,7 @@
         <v>#REF!</v>
       </c>
       <c r="F807" s="29" t="e">
-        <f>LOOKUP("Goal", EventLog!#REF!, EventLog!Q4:Q9)</f>
+        <f>LOOKUP("Goal", EventLog!#REF!, EventLog!O4:O9)</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -30502,30 +30381,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="J1" s="57" t="s">
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="O1" s="54" t="s">
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="O1" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="15"/>

</xml_diff>